<commit_message>
Added pins for LCD.Keypad
Using 4-Bit variation
</commit_message>
<xml_diff>
--- a/ArduinoPinout.xlsx
+++ b/ArduinoPinout.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudie/Documents/Projekte/PasswordKeypad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YowHwuiLow/Documents/Arduino/PasswordKeypad/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
   <si>
     <t>Arduino Pinout</t>
   </si>
@@ -249,6 +252,9 @@
   </si>
   <si>
     <t>Keypad</t>
+  </si>
+  <si>
+    <t>LCD.Keypad</t>
   </si>
 </sst>
 </file>
@@ -327,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -605,7 +611,7 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,30 +717,66 @@
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
trigger Led Entfernt (#20)
Trigger Led entfernt und wie Progress LED Pins umgelegt
</commit_message>
<xml_diff>
--- a/ArduinoPinout.xlsx
+++ b/ArduinoPinout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="131">
   <si>
     <t>Arduino Pinout</t>
   </si>
@@ -327,9 +327,6 @@
   </si>
   <si>
     <t>Farbsensor.LEDgruen</t>
-  </si>
-  <si>
-    <t>Farbsensor.trigger</t>
   </si>
   <si>
     <t>Farbsensor.progressLED1</t>
@@ -463,7 +460,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +506,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +583,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -596,6 +599,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -901,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,7 +1013,7 @@
         <v>69</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1023,7 +1027,7 @@
         <v>69</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1286,8 +1290,8 @@
       <c r="B32" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>99</v>
+      <c r="C32" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1297,8 +1301,8 @@
       <c r="B33" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>100</v>
+      <c r="C33" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1308,8 +1312,8 @@
       <c r="B34" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>101</v>
+      <c r="C34" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1319,8 +1323,8 @@
       <c r="B35" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C35" t="s">
-        <v>102</v>
+      <c r="C35" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1330,20 +1334,15 @@
       <c r="B36" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C36" t="s">
-        <v>103</v>
+      <c r="C36" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
-      </c>
+      <c r="B37" s="15"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
@@ -1353,7 +1352,7 @@
         <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1364,7 +1363,7 @@
         <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1375,7 +1374,7 @@
         <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1386,7 +1385,7 @@
         <v>68</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1397,7 +1396,7 @@
         <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1408,7 +1407,7 @@
         <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1419,7 +1418,7 @@
         <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1430,7 +1429,7 @@
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1441,7 +1440,7 @@
         <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1452,7 +1451,7 @@
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1463,7 +1462,7 @@
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1474,7 +1473,7 @@
         <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1485,7 +1484,7 @@
         <v>68</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1496,7 +1495,7 @@
         <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1507,7 +1506,7 @@
         <v>68</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1518,7 +1517,7 @@
         <v>68</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1529,7 +1528,7 @@
         <v>68</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1540,12 +1539,12 @@
         <v>68</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>68</v>
@@ -1556,7 +1555,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>68</v>
@@ -1567,29 +1566,29 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>